<commit_message>
Add locus IDs to GenBank sequences based on phylogenetic clustering with named ERVs
</commit_message>
<xml_diff>
--- a/tabular/erv/erv-curated-side-data.xlsx
+++ b/tabular/erv/erv-curated-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/Retrovirus/Lentivirus-GLUE/tabular/erv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21012CE-3D47-994A-BEFF-A3F583E72A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612EB68F-899E-6248-8272-182B2AD36F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22300" yWindow="4840" windowWidth="27240" windowHeight="16440" xr2:uid="{5FE1C2E0-EA86-3840-B2CC-A8C1F65F9AD7}"/>
+    <workbookView xWindow="17140" yWindow="5760" windowWidth="27240" windowHeight="16440" xr2:uid="{5FE1C2E0-EA86-3840-B2CC-A8C1F65F9AD7}"/>
   </bookViews>
   <sheets>
     <sheet name="erv-loci" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="168">
   <si>
     <t>FJ707322</t>
   </si>
@@ -145,9 +145,6 @@
     <t>FJ707357</t>
   </si>
   <si>
-    <t>FJ707358</t>
-  </si>
-  <si>
     <t>FJ707359</t>
   </si>
   <si>
@@ -512,6 +509,36 @@
   </si>
   <si>
     <t>sequence_length</t>
+  </si>
+  <si>
+    <t>locus_structure</t>
+  </si>
+  <si>
+    <t>Gag</t>
+  </si>
+  <si>
+    <t>LTR</t>
+  </si>
+  <si>
+    <t>Pol</t>
+  </si>
+  <si>
+    <t>env-rev</t>
+  </si>
+  <si>
+    <t>Pol-Vif-Env</t>
+  </si>
+  <si>
+    <t>Gag-Pol</t>
+  </si>
+  <si>
+    <t>Env</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>NK</t>
   </si>
 </sst>
 </file>
@@ -567,9 +594,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -884,2067 +917,2764 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC27A048-80C5-F84C-A42A-BAF0C66D1548}">
-  <dimension ref="A1:F120"/>
+  <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G119" sqref="A1:G119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
     <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
         <v>154</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>134</v>
-      </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="E2">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3210</v>
+      </c>
+      <c r="F2" s="3">
+        <v>126</v>
+      </c>
+      <c r="G2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="D3" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="E3">
-        <v>2881</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2879</v>
+      </c>
+      <c r="F3" s="3">
+        <v>127</v>
+      </c>
+      <c r="G3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="E4">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2879</v>
+      </c>
+      <c r="F4" s="3">
+        <v>128</v>
+      </c>
+      <c r="G4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="D5" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="E5">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2873</v>
+      </c>
+      <c r="F5" s="3">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6">
+        <v>2784</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>42</v>
       </c>
-      <c r="B6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E6">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="E7">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1128</v>
+      </c>
+      <c r="F7" s="3">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>154</v>
       </c>
       <c r="C8" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="E8">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1118</v>
+      </c>
+      <c r="F8" s="3">
+        <v>125</v>
+      </c>
+      <c r="G8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9">
+        <v>1067</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10">
+        <v>605</v>
+      </c>
+      <c r="F10" s="3">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D11" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E11">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>902</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="D12" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E12">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>902</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C13" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E13">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>902</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C14" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E14">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>902</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C15" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D15" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E15">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>901</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E16">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>883</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D17" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E17">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C18" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D18" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E18">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C19" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D19" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E19">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C20" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D20" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E20">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G20" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C21" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D21" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E21">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G21" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C22" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D22" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E22">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G22" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C23" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E23">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C24" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D24" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E24">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C25" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D25" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E25">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G25" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C26" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D26" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E26">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C27" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D27" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E27">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C28" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D28" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E28">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B29" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D29" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E29">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G29" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C30" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E30">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G30" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C31" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E31">
-        <v>1286</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G31" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C32" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E32">
-        <v>1287</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G32" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C33" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D33" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E33">
-        <v>1068</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G33" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C34" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E34">
-        <v>1260</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G34" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C35" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E35">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G35" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C36" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E36">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G36" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C37" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E37">
-        <v>1437</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G37" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C38" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E38">
-        <v>1437</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G38" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>114</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C39" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E39">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G39" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C40" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="D40" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E40">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>119</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C41" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="D41" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E41">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G41" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D42" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E42">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G42" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>121</v>
       </c>
       <c r="B43" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C43" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D43" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E43">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G43" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>123</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D44" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E44">
-        <v>2165</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>880</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G44" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="B45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C45" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E45">
         <v>880</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G45" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>125</v>
       </c>
       <c r="B46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C46" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E46">
         <v>880</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="B47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C47" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E47">
         <v>880</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G47" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" t="s">
+        <v>149</v>
+      </c>
+      <c r="D48" t="s">
+        <v>130</v>
+      </c>
+      <c r="E48">
+        <v>880</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G48" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>129</v>
+      </c>
+      <c r="B49" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" t="s">
+        <v>149</v>
+      </c>
+      <c r="D49" t="s">
+        <v>130</v>
+      </c>
+      <c r="E49">
+        <v>880</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G49" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" t="s">
+        <v>130</v>
+      </c>
+      <c r="C50" t="s">
+        <v>143</v>
+      </c>
+      <c r="D50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50">
+        <v>879</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G50" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>67</v>
       </c>
-      <c r="B48" t="s">
-        <v>131</v>
-      </c>
-      <c r="C48" t="s">
-        <v>144</v>
-      </c>
-      <c r="D48" t="s">
-        <v>131</v>
-      </c>
-      <c r="E48">
+      <c r="B51" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" t="s">
+        <v>130</v>
+      </c>
+      <c r="E51">
         <v>879</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>68</v>
-      </c>
-      <c r="B49" t="s">
-        <v>131</v>
-      </c>
-      <c r="C49" t="s">
-        <v>144</v>
-      </c>
-      <c r="D49" t="s">
-        <v>131</v>
-      </c>
-      <c r="E49">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>69</v>
-      </c>
-      <c r="B50" t="s">
-        <v>131</v>
-      </c>
-      <c r="C50" t="s">
-        <v>144</v>
-      </c>
-      <c r="D50" t="s">
-        <v>131</v>
-      </c>
-      <c r="E50">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>70</v>
-      </c>
-      <c r="B51" t="s">
-        <v>131</v>
-      </c>
-      <c r="C51" t="s">
-        <v>144</v>
-      </c>
-      <c r="D51" t="s">
-        <v>131</v>
-      </c>
-      <c r="E51">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G51" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C52" t="s">
         <v>144</v>
       </c>
       <c r="D52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E52">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <v>879</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G52" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="B53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C53" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E53">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+        <v>879</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G53" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="B54" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C54" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D54" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E54">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+        <v>878</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G54" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>127</v>
       </c>
       <c r="B55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C55" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E55">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>878</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G55" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B56" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C56" t="s">
         <v>145</v>
       </c>
       <c r="D56" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E56">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+        <v>877</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G56" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B57" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C57" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D57" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E57">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+        <v>875</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G57" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="B58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C58" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E58">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+        <v>874</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G58" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="B59" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C59" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D59" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E59">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+        <v>874</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G59" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="B60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C60" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E60">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+        <v>874</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G60" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="B61" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C61" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D61" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E61">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+        <v>874</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G61" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B62" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C62" t="s">
         <v>145</v>
       </c>
       <c r="D62" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E62">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+        <v>873</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G62" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B63" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C63" t="s">
         <v>145</v>
       </c>
       <c r="D63" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E63">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+        <v>873</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G63" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>102</v>
+      </c>
+      <c r="B64" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" t="s">
+        <v>147</v>
+      </c>
+      <c r="D64" t="s">
+        <v>130</v>
+      </c>
+      <c r="E64">
+        <v>873</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G64" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>104</v>
+      </c>
+      <c r="B65" t="s">
+        <v>130</v>
+      </c>
+      <c r="C65" t="s">
+        <v>147</v>
+      </c>
+      <c r="D65" t="s">
+        <v>130</v>
+      </c>
+      <c r="E65">
+        <v>873</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G65" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>106</v>
+      </c>
+      <c r="B66" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" t="s">
+        <v>147</v>
+      </c>
+      <c r="D66" t="s">
+        <v>130</v>
+      </c>
+      <c r="E66">
+        <v>873</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G66" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>76</v>
+      </c>
+      <c r="B67" t="s">
+        <v>130</v>
+      </c>
+      <c r="C67" t="s">
+        <v>144</v>
+      </c>
+      <c r="D67" t="s">
+        <v>130</v>
+      </c>
+      <c r="E67">
+        <v>860</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G67" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" t="s">
+        <v>144</v>
+      </c>
+      <c r="D68" t="s">
+        <v>130</v>
+      </c>
+      <c r="E68">
+        <v>860</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G68" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>82</v>
+      </c>
+      <c r="B69" t="s">
+        <v>130</v>
+      </c>
+      <c r="C69" t="s">
+        <v>145</v>
+      </c>
+      <c r="D69" t="s">
+        <v>130</v>
+      </c>
+      <c r="E69">
+        <v>837</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G69" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>83</v>
       </c>
-      <c r="B64" t="s">
-        <v>131</v>
-      </c>
-      <c r="C64" t="s">
-        <v>146</v>
-      </c>
-      <c r="D64" t="s">
-        <v>131</v>
-      </c>
-      <c r="E64">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>84</v>
-      </c>
-      <c r="B65" t="s">
-        <v>131</v>
-      </c>
-      <c r="C65" t="s">
-        <v>146</v>
-      </c>
-      <c r="D65" t="s">
-        <v>131</v>
-      </c>
-      <c r="E65">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>85</v>
-      </c>
-      <c r="B66" t="s">
-        <v>131</v>
-      </c>
-      <c r="C66" t="s">
-        <v>146</v>
-      </c>
-      <c r="D66" t="s">
-        <v>131</v>
-      </c>
-      <c r="E66">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>86</v>
-      </c>
-      <c r="B67" t="s">
-        <v>131</v>
-      </c>
-      <c r="C67" t="s">
-        <v>146</v>
-      </c>
-      <c r="D67" t="s">
-        <v>131</v>
-      </c>
-      <c r="E67">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>87</v>
-      </c>
-      <c r="B68" t="s">
-        <v>131</v>
-      </c>
-      <c r="C68" t="s">
-        <v>146</v>
-      </c>
-      <c r="D68" t="s">
-        <v>131</v>
-      </c>
-      <c r="E68">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>88</v>
-      </c>
-      <c r="B69" t="s">
-        <v>131</v>
-      </c>
-      <c r="C69" t="s">
-        <v>146</v>
-      </c>
-      <c r="D69" t="s">
-        <v>131</v>
-      </c>
-      <c r="E69">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>89</v>
-      </c>
       <c r="B70" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C70" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D70" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E70">
         <v>837</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G70" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C71" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E71">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+        <v>837</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G71" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C72" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E72">
         <v>837</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G72" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B73" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C73" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D73" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E73">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+        <v>837</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G73" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B74" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C74" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D74" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E74">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+        <v>837</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G74" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B75" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C75" t="s">
         <v>147</v>
       </c>
       <c r="D75" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E75">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+        <v>837</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G75" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="B76" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C76" t="s">
         <v>147</v>
       </c>
       <c r="D76" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E76">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+        <v>837</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G76" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="B77" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C77" t="s">
         <v>147</v>
       </c>
       <c r="D77" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E77">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+        <v>837</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G77" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="B78" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C78" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D78" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E78">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2165</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G78" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="B79" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C79" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D79" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E79">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G79" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="B80" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C80" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D80" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E80">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G80" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="B81" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C81" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D81" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E81">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G81" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>101</v>
+        <v>21</v>
       </c>
       <c r="B82" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C82" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D82" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E82">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G82" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="B83" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C83" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D83" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E83">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G83" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>103</v>
+        <v>5</v>
       </c>
       <c r="B84" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C84" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="D84" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E84">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G84" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>104</v>
+        <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C85" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D85" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E85">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G85" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="B86" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C86" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D86" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E86">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G86" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="B87" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C87" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D87" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E87">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G87" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="B88" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C88" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D88" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E88">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G88" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C89" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D89" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E89">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G89" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>109</v>
+        <v>18</v>
       </c>
       <c r="B90" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C90" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D90" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E90">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G90" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>110</v>
+        <v>19</v>
       </c>
       <c r="B91" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C91" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D91" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E91">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G91" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>111</v>
+        <v>22</v>
       </c>
       <c r="B92" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C92" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D92" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E92">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G92" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="B93" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C93" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D93" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E93">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G93" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="B94" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C94" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D94" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E94">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G94" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="B95" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C95" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="D95" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E95">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G95" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="B96" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C96" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D96" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E96">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G96" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
       <c r="B97" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C97" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="D97" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E97">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G97" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="B98" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C98" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D98" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="E98">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1437</v>
+      </c>
+      <c r="F98" s="3">
+        <v>1</v>
+      </c>
+      <c r="G98" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="B99" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C99" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D99" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="E99">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1437</v>
+      </c>
+      <c r="F99" s="3">
+        <v>1</v>
+      </c>
+      <c r="G99" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="B100" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C100" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D100" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="E100">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1380</v>
+      </c>
+      <c r="F100" s="3">
+        <v>1</v>
+      </c>
+      <c r="G100" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>120</v>
+        <v>25</v>
       </c>
       <c r="B101" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C101" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D101" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="E101">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1287</v>
+      </c>
+      <c r="F101" s="3">
+        <v>1</v>
+      </c>
+      <c r="G101" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>121</v>
+        <v>24</v>
       </c>
       <c r="B102" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C102" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D102" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="E102">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1286</v>
+      </c>
+      <c r="F102" s="3">
+        <v>1</v>
+      </c>
+      <c r="G102" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>122</v>
+        <v>27</v>
       </c>
       <c r="B103" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C103" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D103" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="E103">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1260</v>
+      </c>
+      <c r="F103" s="3">
+        <v>1</v>
+      </c>
+      <c r="G103" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>123</v>
+        <v>23</v>
       </c>
       <c r="B104" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C104" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D104" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="E104">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1125</v>
+      </c>
+      <c r="F104" s="3">
+        <v>1</v>
+      </c>
+      <c r="G104" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>124</v>
+        <v>26</v>
       </c>
       <c r="B105" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C105" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D105" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="E105">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1068</v>
+      </c>
+      <c r="F105" s="3">
+        <v>1</v>
+      </c>
+      <c r="G105" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>125</v>
+        <v>34</v>
       </c>
       <c r="B106" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C106" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D106" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="E106">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1024</v>
+      </c>
+      <c r="F106" s="3">
+        <v>1</v>
+      </c>
+      <c r="G106" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>126</v>
+        <v>35</v>
       </c>
       <c r="B107" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C107" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D107" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="E107">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1024</v>
+      </c>
+      <c r="F107" s="3">
+        <v>1</v>
+      </c>
+      <c r="G107" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="B108" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C108" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D108" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="E108">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+        <v>730</v>
+      </c>
+      <c r="F108" s="3">
+        <v>1</v>
+      </c>
+      <c r="G108" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>128</v>
+        <v>33</v>
       </c>
       <c r="B109" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C109" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D109" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="E109">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+        <v>729</v>
+      </c>
+      <c r="F109" s="3">
+        <v>1</v>
+      </c>
+      <c r="G109" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>129</v>
+        <v>29</v>
       </c>
       <c r="B110" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C110" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D110" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="E110">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+        <v>706</v>
+      </c>
+      <c r="F110" s="3">
+        <v>1</v>
+      </c>
+      <c r="G110" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>130</v>
+        <v>3</v>
       </c>
       <c r="B111" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C111" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D111" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="E111">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G111" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="B112" t="s">
-        <v>155</v>
+        <v>52</v>
       </c>
       <c r="C112" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="D112" t="s">
-        <v>152</v>
+        <v>52</v>
       </c>
       <c r="E112">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G112" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="B113" t="s">
-        <v>155</v>
+        <v>52</v>
       </c>
       <c r="C113" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="D113" t="s">
-        <v>152</v>
+        <v>52</v>
       </c>
       <c r="E113">
-        <v>2873</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G113" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="B114" t="s">
-        <v>155</v>
+        <v>52</v>
       </c>
       <c r="C114" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="D114" t="s">
-        <v>152</v>
+        <v>52</v>
       </c>
       <c r="E114">
-        <v>2879</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G114" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B115" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="C115" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="D115" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="E115">
-        <v>2879</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2881</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G115" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B116" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="C116" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="D116" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="E116">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2019</v>
+      </c>
+      <c r="F116" s="3">
+        <v>72</v>
+      </c>
+      <c r="G116" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B117" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="C117" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="D117" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="E117">
-        <v>2784</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+        <v>787</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G117" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B118" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="C118" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="D118" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="E118">
-        <v>3210</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+        <v>681</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G118" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B119" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="C119" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="D119" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="E119">
-        <v>1118</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>51</v>
-      </c>
-      <c r="B120" t="s">
-        <v>155</v>
-      </c>
-      <c r="C120" t="s">
-        <v>151</v>
-      </c>
-      <c r="D120" t="s">
-        <v>152</v>
-      </c>
-      <c r="E120">
-        <v>605</v>
+        <v>397</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G119" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D120">
-    <sortCondition ref="A2:A120"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G119">
+    <sortCondition ref="B2:B119"/>
+    <sortCondition descending="1" ref="E2:E119"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2960,112 +3690,112 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>